<commit_message>
Construção de gráficos com plages
</commit_message>
<xml_diff>
--- a/Exoplanets/55Cnc_e/Parâmetros.xlsx
+++ b/Exoplanets/55Cnc_e/Parâmetros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\StarsAndExoplanets\Exoplanets\55Cnc_e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6533BE67-A0EF-455F-AA30-5D7FDC984A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2BEE7A-EE41-4036-8C46-519A1B2A1505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="3105" windowWidth="13785" windowHeight="11325" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -367,7 +378,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -440,6 +451,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -766,32 +780,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64130676-9D84-4B43-9CC6-731DFC23A473}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" customWidth="1"/>
+    <col min="21" max="21" width="11.5546875" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B1" s="16" t="s">
         <v>44</v>
       </c>
@@ -865,7 +879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>45</v>
       </c>
@@ -888,16 +902,17 @@
         <v>0</v>
       </c>
       <c r="I2" s="17">
-        <v>0</v>
-      </c>
-      <c r="J2" s="18">
+        <v>1</v>
+      </c>
+      <c r="J2" s="26">
         <v>0.1</v>
       </c>
-      <c r="K2" s="18">
-        <v>0</v>
-      </c>
-      <c r="L2" s="18">
-        <v>0.2</v>
+      <c r="K2" s="26">
+        <v>40</v>
+      </c>
+      <c r="L2" s="26">
+        <f>SQRT(0.1)</f>
+        <v>0.31622776601683794</v>
       </c>
       <c r="M2" s="19">
         <v>2</v>
@@ -939,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -947,9 +962,16 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="J3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="26">
+        <v>-40</v>
+      </c>
+      <c r="L3" s="26">
+        <f>SQRT(0.1)</f>
+        <v>0.31622776601683794</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -965,7 +987,7 @@
         <v>0.28284271249999998</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -973,9 +995,16 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="J4" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="26">
+        <v>0</v>
+      </c>
+      <c r="L4" s="26">
+        <f>SQRT(0.1)</f>
+        <v>0.31622776601683794</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -988,7 +1017,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -996,9 +1025,9 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1011,7 +1040,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1019,9 +1048,9 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1034,7 +1063,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1057,7 +1086,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1080,7 +1109,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1103,7 +1132,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1126,7 +1155,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1149,7 +1178,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1161,107 +1190,107 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>40</v>
       </c>

</xml_diff>